<commit_message>
Update data to include Oct 2015 data
</commit_message>
<xml_diff>
--- a/data/turvapaikanhakijamäärät.xlsx
+++ b/data/turvapaikanhakijamäärät.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16360" windowHeight="17220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Maakoodi</t>
   </si>
@@ -193,13 +193,16 @@
   </si>
   <si>
     <t xml:space="preserve">XKX </t>
+  </si>
+  <si>
+    <t>NGA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,21 +226,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="dashed">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="dashed">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="dashed">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -246,9 +275,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -523,7 +555,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -531,13 +563,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BH57"/>
+  <dimension ref="A1:BH58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A44" sqref="A44:XFD44"/>
+      <selection pane="bottomRight" activeCell="BG58" sqref="BG58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -886,6 +918,9 @@
       <c r="BF2">
         <v>188</v>
       </c>
+      <c r="BG2" s="2">
+        <v>390</v>
+      </c>
     </row>
     <row r="3" spans="1:60">
       <c r="A3" t="s">
@@ -914,6 +949,9 @@
       </c>
       <c r="BF3">
         <v>2</v>
+      </c>
+      <c r="BG3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:60">
@@ -977,6 +1015,9 @@
       <c r="BE4">
         <v>1</v>
       </c>
+      <c r="BG4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:60">
       <c r="A5" t="s">
@@ -1083,6 +1124,9 @@
       <c r="BF9">
         <v>5</v>
       </c>
+      <c r="BG9">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:60">
       <c r="A10" t="s">
@@ -1108,6 +1152,9 @@
       <c r="BF11">
         <v>1</v>
       </c>
+      <c r="BG11">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:60">
       <c r="A12" t="s">
@@ -1143,6 +1190,9 @@
       <c r="BF12">
         <v>2</v>
       </c>
+      <c r="BG12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:60">
       <c r="A13" t="s">
@@ -1248,7 +1298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:58">
+    <row r="17" spans="1:59">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1360,8 +1410,11 @@
       <c r="BF17">
         <v>243</v>
       </c>
-    </row>
-    <row r="18" spans="1:58">
+      <c r="BG17">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:59">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1369,7 +1422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:58">
+    <row r="19" spans="1:59">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1400,8 +1453,11 @@
       <c r="BF19">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:58">
+      <c r="BG19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:59">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1411,8 +1467,11 @@
       <c r="BF20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:58">
+      <c r="BG20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:59">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1438,7 +1497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:58">
+    <row r="22" spans="1:59">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1452,7 +1511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:58">
+    <row r="23" spans="1:59">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1463,7 +1522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:58">
+    <row r="24" spans="1:59">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1471,7 +1530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:58">
+    <row r="25" spans="1:59">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1530,7 +1589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:58">
+    <row r="26" spans="1:59">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1541,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:58">
+    <row r="27" spans="1:59">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -1549,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:58">
+    <row r="28" spans="1:59">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1563,7 +1622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:58">
+    <row r="29" spans="1:59">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -1577,7 +1636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:58">
+    <row r="30" spans="1:59">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1605,8 +1664,11 @@
       <c r="BF30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:58">
+      <c r="BG30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:59">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -1623,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:58">
+    <row r="32" spans="1:59">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -1690,8 +1752,11 @@
       <c r="BF32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:58">
+      <c r="BG32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:59">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1699,7 +1764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:58">
+    <row r="34" spans="1:59">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -1707,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:58">
+    <row r="35" spans="1:59">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -1721,539 +1786,568 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:58">
+    <row r="36" spans="1:59">
       <c r="A36" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="AH36">
+        <v>1</v>
+      </c>
+      <c r="AO36">
+        <v>1</v>
+      </c>
+      <c r="AR36">
+        <v>1</v>
+      </c>
+      <c r="BG36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:59">
+      <c r="A37" t="s">
         <v>20</v>
       </c>
-      <c r="BE36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:58">
-      <c r="A37" t="s">
+      <c r="BE37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:59">
+      <c r="A38" t="s">
         <v>48</v>
       </c>
-      <c r="AI37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:58">
-      <c r="A38" t="s">
+      <c r="AI38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:59">
+      <c r="A39" t="s">
         <v>21</v>
       </c>
-      <c r="U38">
-        <v>1</v>
-      </c>
-      <c r="AK38">
-        <v>1</v>
-      </c>
-      <c r="AT38">
-        <v>1</v>
-      </c>
-      <c r="AV38">
-        <v>2</v>
-      </c>
-      <c r="BF38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:58">
-      <c r="A39" t="s">
+      <c r="U39">
+        <v>1</v>
+      </c>
+      <c r="AK39">
+        <v>1</v>
+      </c>
+      <c r="AT39">
+        <v>1</v>
+      </c>
+      <c r="AV39">
+        <v>2</v>
+      </c>
+      <c r="BF39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:59">
+      <c r="A40" t="s">
         <v>49</v>
       </c>
-      <c r="O39">
-        <v>1</v>
-      </c>
-      <c r="W39">
-        <v>1</v>
-      </c>
-      <c r="AD39">
-        <v>1</v>
-      </c>
-      <c r="AF39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:58">
-      <c r="A40" t="s">
+      <c r="O40">
+        <v>1</v>
+      </c>
+      <c r="W40">
+        <v>1</v>
+      </c>
+      <c r="AD40">
+        <v>1</v>
+      </c>
+      <c r="AF40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:59">
+      <c r="A41" t="s">
         <v>22</v>
       </c>
-      <c r="N40">
-        <v>1</v>
-      </c>
-      <c r="S40">
-        <v>1</v>
-      </c>
-      <c r="T40">
-        <v>1</v>
-      </c>
-      <c r="AA40">
-        <v>1</v>
-      </c>
-      <c r="AM40">
-        <v>1</v>
-      </c>
-      <c r="AZ40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:58">
-      <c r="A41" t="s">
+      <c r="N41">
+        <v>1</v>
+      </c>
+      <c r="S41">
+        <v>1</v>
+      </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
+      <c r="AA41">
+        <v>1</v>
+      </c>
+      <c r="AM41">
+        <v>1</v>
+      </c>
+      <c r="AZ41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:59">
+      <c r="A42" t="s">
         <v>23</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
         <v>7</v>
       </c>
-      <c r="D41">
+      <c r="D42">
         <v>8</v>
       </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="F41">
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
         <v>6</v>
       </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-      <c r="H41">
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
         <v>4</v>
       </c>
-      <c r="I41">
+      <c r="I42">
         <v>8</v>
       </c>
-      <c r="J41">
+      <c r="J42">
         <v>4</v>
       </c>
-      <c r="K41">
-        <v>2</v>
-      </c>
-      <c r="L41">
-        <v>1</v>
-      </c>
-      <c r="M41">
-        <v>2</v>
-      </c>
-      <c r="N41">
-        <v>2</v>
-      </c>
-      <c r="O41">
-        <v>1</v>
-      </c>
-      <c r="P41">
-        <v>1</v>
-      </c>
-      <c r="Q41">
-        <v>1</v>
-      </c>
-      <c r="S41">
-        <v>3</v>
-      </c>
-      <c r="T41">
-        <v>1</v>
-      </c>
-      <c r="U41">
-        <v>3</v>
-      </c>
-      <c r="V41">
+      <c r="K42">
+        <v>2</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>2</v>
+      </c>
+      <c r="N42">
+        <v>2</v>
+      </c>
+      <c r="O42">
+        <v>1</v>
+      </c>
+      <c r="P42">
+        <v>1</v>
+      </c>
+      <c r="Q42">
+        <v>1</v>
+      </c>
+      <c r="S42">
+        <v>3</v>
+      </c>
+      <c r="T42">
+        <v>1</v>
+      </c>
+      <c r="U42">
+        <v>3</v>
+      </c>
+      <c r="V42">
         <v>6</v>
       </c>
-      <c r="W41">
+      <c r="W42">
         <v>7</v>
       </c>
-      <c r="X41">
-        <v>3</v>
-      </c>
-      <c r="Y41">
-        <v>2</v>
-      </c>
-      <c r="Z41">
+      <c r="X42">
+        <v>3</v>
+      </c>
+      <c r="Y42">
+        <v>2</v>
+      </c>
+      <c r="Z42">
         <v>6</v>
       </c>
-      <c r="AA41">
-        <v>2</v>
-      </c>
-      <c r="AB41">
+      <c r="AA42">
+        <v>2</v>
+      </c>
+      <c r="AB42">
         <v>5</v>
       </c>
-      <c r="AC41">
+      <c r="AC42">
         <v>4</v>
       </c>
-      <c r="AD41">
-        <v>3</v>
-      </c>
-      <c r="AE41">
-        <v>2</v>
-      </c>
-      <c r="AF41">
+      <c r="AD42">
+        <v>3</v>
+      </c>
+      <c r="AE42">
+        <v>2</v>
+      </c>
+      <c r="AF42">
         <v>4</v>
       </c>
-      <c r="AG41">
-        <v>3</v>
-      </c>
-      <c r="AH41">
-        <v>1</v>
-      </c>
-      <c r="AI41">
-        <v>2</v>
-      </c>
-      <c r="AJ41">
-        <v>1</v>
-      </c>
-      <c r="AK41">
-        <v>3</v>
-      </c>
-      <c r="AL41">
+      <c r="AG42">
+        <v>3</v>
+      </c>
+      <c r="AH42">
+        <v>1</v>
+      </c>
+      <c r="AI42">
+        <v>2</v>
+      </c>
+      <c r="AJ42">
+        <v>1</v>
+      </c>
+      <c r="AK42">
+        <v>3</v>
+      </c>
+      <c r="AL42">
         <v>4</v>
       </c>
-      <c r="AM41">
-        <v>1</v>
-      </c>
-      <c r="AN41">
-        <v>3</v>
-      </c>
-      <c r="AO41">
-        <v>1</v>
-      </c>
-      <c r="AP41">
-        <v>1</v>
-      </c>
-      <c r="AQ41">
+      <c r="AM42">
+        <v>1</v>
+      </c>
+      <c r="AN42">
+        <v>3</v>
+      </c>
+      <c r="AO42">
+        <v>1</v>
+      </c>
+      <c r="AP42">
+        <v>1</v>
+      </c>
+      <c r="AQ42">
         <v>5</v>
       </c>
-      <c r="AR41">
+      <c r="AR42">
         <v>5</v>
       </c>
-      <c r="AS41">
+      <c r="AS42">
         <v>9</v>
       </c>
-      <c r="AT41">
+      <c r="AT42">
         <v>6</v>
       </c>
-      <c r="AU41">
+      <c r="AU42">
         <v>5</v>
       </c>
-      <c r="AV41">
+      <c r="AV42">
         <v>6</v>
       </c>
-      <c r="AW41">
-        <v>2</v>
-      </c>
-      <c r="AX41">
+      <c r="AW42">
+        <v>2</v>
+      </c>
+      <c r="AX42">
         <v>5</v>
       </c>
-      <c r="AY41">
+      <c r="AY42">
         <v>9</v>
       </c>
-      <c r="AZ41">
+      <c r="AZ42">
         <v>11</v>
       </c>
-      <c r="BA41">
+      <c r="BA42">
         <v>9</v>
       </c>
-      <c r="BB41">
+      <c r="BB42">
         <v>23</v>
       </c>
-      <c r="BC41">
+      <c r="BC42">
         <v>20</v>
       </c>
-      <c r="BD41">
+      <c r="BD42">
         <v>38</v>
       </c>
-      <c r="BE41">
+      <c r="BE42">
         <v>40</v>
       </c>
-      <c r="BF41">
+      <c r="BF42">
         <v>69</v>
       </c>
-    </row>
-    <row r="42" spans="1:58">
-      <c r="A42" t="s">
+      <c r="BG42">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:59">
+      <c r="A43" t="s">
         <v>50</v>
       </c>
-      <c r="AD42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:58">
-      <c r="A43" t="s">
+      <c r="AD43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:59">
+      <c r="A44" t="s">
         <v>24</v>
       </c>
-      <c r="BD43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:58">
-      <c r="A44" t="s">
+      <c r="BD44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:59">
+      <c r="A45" t="s">
         <v>25</v>
       </c>
-      <c r="C44">
-        <v>2</v>
-      </c>
-      <c r="I44">
-        <v>1</v>
-      </c>
-      <c r="J44">
-        <v>1</v>
-      </c>
-      <c r="P44">
-        <v>1</v>
-      </c>
-      <c r="U44">
-        <v>1</v>
-      </c>
-      <c r="AF44">
-        <v>1</v>
-      </c>
-      <c r="AJ44">
-        <v>1</v>
-      </c>
-      <c r="AM44">
-        <v>1</v>
-      </c>
-      <c r="AN44">
-        <v>1</v>
-      </c>
-      <c r="AO44">
-        <v>1</v>
-      </c>
-      <c r="AR44">
-        <v>1</v>
-      </c>
-      <c r="AU44">
-        <v>2</v>
-      </c>
-      <c r="AX44">
-        <v>1</v>
-      </c>
-      <c r="BA44">
-        <v>1</v>
-      </c>
-      <c r="BB44">
-        <v>1</v>
-      </c>
-      <c r="BC44">
-        <v>1</v>
-      </c>
-      <c r="BD44">
-        <v>1</v>
-      </c>
-      <c r="BE44">
-        <v>2</v>
-      </c>
-      <c r="BF44">
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="P45">
+        <v>1</v>
+      </c>
+      <c r="U45">
+        <v>1</v>
+      </c>
+      <c r="AF45">
+        <v>1</v>
+      </c>
+      <c r="AJ45">
+        <v>1</v>
+      </c>
+      <c r="AM45">
+        <v>1</v>
+      </c>
+      <c r="AN45">
+        <v>1</v>
+      </c>
+      <c r="AO45">
+        <v>1</v>
+      </c>
+      <c r="AR45">
+        <v>1</v>
+      </c>
+      <c r="AU45">
+        <v>2</v>
+      </c>
+      <c r="AX45">
+        <v>1</v>
+      </c>
+      <c r="BA45">
+        <v>1</v>
+      </c>
+      <c r="BB45">
+        <v>1</v>
+      </c>
+      <c r="BC45">
+        <v>1</v>
+      </c>
+      <c r="BD45">
+        <v>1</v>
+      </c>
+      <c r="BE45">
+        <v>2</v>
+      </c>
+      <c r="BF45">
         <v>8</v>
       </c>
-    </row>
-    <row r="45" spans="1:58">
-      <c r="A45" t="s">
+      <c r="BG45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:59">
+      <c r="A46" t="s">
         <v>38</v>
       </c>
-      <c r="AC45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:58">
-      <c r="A46" t="s">
+      <c r="AC46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:59">
+      <c r="A47" t="s">
         <v>30</v>
       </c>
-      <c r="I46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:58">
-      <c r="A47" t="s">
+      <c r="I47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:59">
+      <c r="A48" t="s">
         <v>31</v>
       </c>
-      <c r="F47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:58">
-      <c r="A48" t="s">
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:59">
+      <c r="A49" t="s">
         <v>26</v>
       </c>
-      <c r="BA48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:58">
-      <c r="A49" t="s">
+      <c r="BA49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:59">
+      <c r="A50" t="s">
         <v>51</v>
       </c>
-      <c r="H49">
-        <v>1</v>
-      </c>
-      <c r="O49">
-        <v>1</v>
-      </c>
-      <c r="W49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:58">
-      <c r="A50" t="s">
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="W50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:59">
+      <c r="A51" t="s">
         <v>27</v>
       </c>
-      <c r="AO50">
-        <v>1</v>
-      </c>
-      <c r="AR50">
+      <c r="AO51">
+        <v>1</v>
+      </c>
+      <c r="AR51">
         <v>5</v>
       </c>
-      <c r="AS50">
-        <v>1</v>
-      </c>
-      <c r="AX50">
-        <v>1</v>
-      </c>
-      <c r="BB50">
-        <v>1</v>
-      </c>
-      <c r="BF50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:58">
-      <c r="A51" t="s">
+      <c r="AS51">
+        <v>1</v>
+      </c>
+      <c r="AX51">
+        <v>1</v>
+      </c>
+      <c r="BB51">
+        <v>1</v>
+      </c>
+      <c r="BF51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:59">
+      <c r="A52" t="s">
         <v>52</v>
       </c>
-      <c r="F51">
-        <v>1</v>
-      </c>
-      <c r="AH51">
-        <v>1</v>
-      </c>
-      <c r="AO51">
-        <v>1</v>
-      </c>
-      <c r="AR51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:58">
-      <c r="A52" t="s">
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="AH52">
+        <v>1</v>
+      </c>
+      <c r="AO52">
+        <v>1</v>
+      </c>
+      <c r="AR52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:59">
+      <c r="A53" t="s">
         <v>32</v>
       </c>
-      <c r="F52">
+      <c r="F53">
         <v>5</v>
       </c>
-      <c r="P52">
-        <v>1</v>
-      </c>
-      <c r="R52">
-        <v>1</v>
-      </c>
-      <c r="S52">
-        <v>1</v>
-      </c>
-      <c r="AB52">
-        <v>1</v>
-      </c>
-      <c r="AC52">
-        <v>1</v>
-      </c>
-      <c r="AI52">
-        <v>1</v>
-      </c>
-      <c r="AJ52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:58">
-      <c r="A53" t="s">
+      <c r="P53">
+        <v>1</v>
+      </c>
+      <c r="R53">
+        <v>1</v>
+      </c>
+      <c r="S53">
+        <v>1</v>
+      </c>
+      <c r="AB53">
+        <v>1</v>
+      </c>
+      <c r="AC53">
+        <v>1</v>
+      </c>
+      <c r="AI53">
+        <v>1</v>
+      </c>
+      <c r="AJ53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:59">
+      <c r="A54" t="s">
         <v>41</v>
       </c>
-      <c r="AO53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:58">
-      <c r="A54" t="s">
+      <c r="AO54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:59">
+      <c r="A55" t="s">
         <v>39</v>
       </c>
-      <c r="AF54">
-        <v>2</v>
-      </c>
-      <c r="AG54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:58">
-      <c r="A55" t="s">
+      <c r="AF55">
+        <v>2</v>
+      </c>
+      <c r="AG55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:59">
+      <c r="A56" t="s">
         <v>53</v>
       </c>
-      <c r="L55">
-        <v>1</v>
-      </c>
-      <c r="S55">
-        <v>3</v>
-      </c>
-      <c r="Y55">
-        <v>1</v>
-      </c>
-      <c r="AE55">
-        <v>1</v>
-      </c>
-      <c r="AG55">
-        <v>1</v>
-      </c>
-      <c r="AZ55">
-        <v>2</v>
-      </c>
-      <c r="BD55">
-        <v>1</v>
-      </c>
-      <c r="BF55">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:58">
-      <c r="A56" t="s">
+      <c r="L56">
+        <v>1</v>
+      </c>
+      <c r="S56">
+        <v>3</v>
+      </c>
+      <c r="Y56">
+        <v>1</v>
+      </c>
+      <c r="AE56">
+        <v>1</v>
+      </c>
+      <c r="AG56">
+        <v>1</v>
+      </c>
+      <c r="AZ56">
+        <v>2</v>
+      </c>
+      <c r="BD56">
+        <v>1</v>
+      </c>
+      <c r="BF56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:59">
+      <c r="A57" t="s">
         <v>54</v>
       </c>
-      <c r="I56">
-        <v>2</v>
-      </c>
-      <c r="S56">
-        <v>1</v>
-      </c>
-      <c r="T56">
-        <v>1</v>
-      </c>
-      <c r="AE56">
-        <v>1</v>
-      </c>
-      <c r="AU56">
-        <v>1</v>
-      </c>
-      <c r="BE56">
-        <v>3</v>
-      </c>
-      <c r="BF56">
+      <c r="I57">
+        <v>2</v>
+      </c>
+      <c r="S57">
+        <v>1</v>
+      </c>
+      <c r="T57">
+        <v>1</v>
+      </c>
+      <c r="AE57">
+        <v>1</v>
+      </c>
+      <c r="AU57">
+        <v>1</v>
+      </c>
+      <c r="BE57">
+        <v>3</v>
+      </c>
+      <c r="BF57">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:58">
-      <c r="A57" t="s">
+      <c r="BG57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:59">
+      <c r="A58" t="s">
         <v>55</v>
       </c>
-      <c r="R57">
-        <v>1</v>
-      </c>
-      <c r="AF57">
-        <v>2</v>
-      </c>
-      <c r="AQ57">
-        <v>1</v>
-      </c>
-      <c r="BE57">
-        <v>1</v>
-      </c>
-      <c r="BF57">
+      <c r="R58">
+        <v>1</v>
+      </c>
+      <c r="AF58">
+        <v>2</v>
+      </c>
+      <c r="AQ58">
+        <v>1</v>
+      </c>
+      <c r="BE58">
+        <v>1</v>
+      </c>
+      <c r="BF58">
         <v>2</v>
       </c>
     </row>

</xml_diff>